<commit_message>
Fix POC pCO2 extraction mismatch
</commit_message>
<xml_diff>
--- a/Ascertainment_Overlap_Intersections.xlsx
+++ b/Ascertainment_Overlap_Intersections.xlsx
@@ -468,13 +468,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>17527</v>
+        <v>8694</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>7659</v>
+        <v>8409</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>5746</v>
+        <v>5059</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>4416</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>3990</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="7">
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>856</v>
+        <v>701</v>
       </c>
     </row>
     <row r="8">
@@ -573,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>481</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>242</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>156</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12">
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update cohort and classifier QA
</commit_message>
<xml_diff>
--- a/Ascertainment_Overlap_Intersections.xlsx
+++ b/Ascertainment_Overlap_Intersections.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>8694</v>
+        <v>4333</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>8409</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="4">
@@ -499,50 +499,50 @@
         <v>0</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>5059</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>2142</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1670</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7">
@@ -550,67 +550,67 @@
         <v>1</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>701</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>438</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>326</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>316</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>129</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>73</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,67 @@
         <v>0</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>18</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove redundant hypercapnia columns
</commit_message>
<xml_diff>
--- a/Ascertainment_Overlap_Intersections.xlsx
+++ b/Ascertainment_Overlap_Intersections.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>UNKNOWN</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>4333</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="3">
@@ -491,29 +491,29 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3041</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1392</v>
+        <v>906</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>536</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>467</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7">
@@ -550,33 +550,33 @@
         <v>1</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>460</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>327</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9">
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>262</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10">
@@ -610,15 +610,15 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>247</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -627,29 +627,29 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>226</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>190</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>184</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>71</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>